<commit_message>
requirement list update 창현
</commit_message>
<xml_diff>
--- a/Requirement List/requriementList_Oh_Changhyun.xlsx
+++ b/Requirement List/requriementList_Oh_Changhyun.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SW_engineering_13_group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SW_engineering_13_group\Requirement List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB39A866-9908-4999-BBEF-3874B1E58B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D1AAB3-AFA3-4239-A450-A11902349B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="1605" windowWidth="21600" windowHeight="11385" xr2:uid="{15D10122-E891-4960-AD69-6842C183E103}"/>
+    <workbookView xWindow="11265" yWindow="0" windowWidth="17535" windowHeight="15600" xr2:uid="{15D10122-E891-4960-AD69-6842C183E103}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>No.</t>
   </si>
@@ -47,52 +47,42 @@
     <t>Use Case</t>
   </si>
   <si>
-    <t>회원은 ID, 비밀번호, 전화번호, 결제 수단, 선호 자전거 유형을 입력하여 회원가입을 할 수 있어야 한다.</t>
-  </si>
-  <si>
     <t>회원가입</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>사용자는 로그인/아웃을 할 수있어야 한다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인/로그아웃</t>
   </si>
   <si>
-    <t>사용자는 탈퇴를 할 수 있어야 한다.</t>
-  </si>
-  <si>
     <t>회원 탈퇴</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>회원은 현재 대여중인 자전거 리스트를 조회할 수 있어야 한다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 대여중인 자전거 리스트 조회</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원은 자전거 대여 정보 조회 화면에서 특정 자전거를 지정된 대여소에 반납할 수 있어야 한다.</t>
-  </si>
-  <si>
-    <t>자전거 반납</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자는 반납할때 원하면 식당추천 및 예약 외부 서비스와 연결되어야 한다.</t>
-  </si>
-  <si>
-    <t>식당 추천 여부</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원은 요금조회 화면에서 대여시간 및 요금을 볼 수 있어야 한다.</t>
-  </si>
-  <si>
     <t>요금 조회</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 로그인, 로그아웃 가능</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원은 ID, 비밀번호, 전화번호, 결제 수단, 선호 자전거 유형을 입력하여 회원가입 가능</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 탈퇴 가능</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원은 요금조회 화면에서 대여시간 및 요금을 확인 가능</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 대여중인 자전거 리스트 조회(+자전거 반납 +식당 추천)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 대여중인 자전거 대여 정보 조회. 대여 정보 조회 리스트에서 특정 자전거를 지정된 대여소에 반납 가능. 반납시 원하면 식당 추천 및 예약 외부 서비스와 연결.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -516,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B74E6A7-CA28-464D-AAD9-9607B7B145D5}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -545,10 +535,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -556,10 +546,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -567,54 +557,32 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
         <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>